<commit_message>
đưa sơ đồ mạch chuyển đổi cổng USB sang TTL
</commit_message>
<xml_diff>
--- a/Docs/ModuleList.xlsx
+++ b/Docs/ModuleList.xlsx
@@ -451,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -513,6 +513,12 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -524,9 +530,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -838,7 +841,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -922,10 +925,10 @@
       <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="25"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
@@ -941,8 +944,8 @@
       <c r="E5" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
@@ -976,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
@@ -1029,7 +1032,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
@@ -1253,10 +1256,10 @@
       <c r="E23" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -1270,8 +1273,8 @@
       <c r="E24" s="14">
         <v>1</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
@@ -1611,14 +1614,14 @@
       <c r="G43" s="7"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-      <c r="C45" s="23"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="21"/>
+      <c r="C46" s="23"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
@@ -1654,17 +1657,17 @@
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="22"/>
+      <c r="C52" s="24"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="22">
+      <c r="B53" s="24">
         <f>1.23*(1+(C51/B51))</f>
         <v>2.73</v>
       </c>
-      <c r="C53" s="22"/>
+      <c r="C53" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
cập nhật tiến trình làm mạch phần cứng
</commit_message>
<xml_diff>
--- a/Docs/ModuleList.xlsx
+++ b/Docs/ModuleList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -841,7 +841,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="7"/>
+      <c r="G12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
@@ -1098,7 +1098,7 @@
       <c r="F14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="7"/>
+      <c r="G14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="21"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14">

</xml_diff>

<commit_message>
đưa lên mạch I2C
</commit_message>
<xml_diff>
--- a/Docs/ModuleList.xlsx
+++ b/Docs/ModuleList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>TT</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>thiếu 1 cái</t>
-  </si>
-  <si>
-    <t>mung lung như một trò đùa :(((</t>
   </si>
   <si>
     <t>chuyển USB vào chung mạch MCU, chuyển Micro SD vào mạch giải mã âm thanh</t>
@@ -451,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -512,6 +509,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -841,7 +841,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -874,7 +874,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,10 +925,10 @@
       <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="22"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
@@ -944,8 +944,8 @@
       <c r="E5" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
@@ -1136,7 +1136,7 @@
       <c r="F16" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="7"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
@@ -1238,7 +1238,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="7"/>
     </row>
@@ -1256,10 +1256,10 @@
       <c r="E23" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -1273,8 +1273,8 @@
       <c r="E24" s="14">
         <v>1</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
@@ -1341,9 +1341,7 @@
       <c r="E28" s="14">
         <v>1</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="F28" s="5"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1360,9 +1358,7 @@
       <c r="E29" s="14">
         <v>2</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="F29" s="5"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1379,9 +1375,7 @@
       <c r="E30" s="14">
         <v>2</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="F30" s="5"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1485,9 +1479,7 @@
       <c r="E36" s="14">
         <v>1</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>99</v>
-      </c>
+      <c r="F36" s="5"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1614,14 +1606,14 @@
       <c r="G43" s="7"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="24"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
@@ -1657,17 +1649,17 @@
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="24"/>
+      <c r="C52" s="25"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="24">
+      <c r="B53" s="25">
         <f>1.23*(1+(C51/B51))</f>
         <v>2.73</v>
       </c>
-      <c r="C53" s="24"/>
+      <c r="C53" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
tải lên các mạch 18 đến 28
</commit_message>
<xml_diff>
--- a/Docs/ModuleList.xlsx
+++ b/Docs/ModuleList.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>TT</t>
   </si>
@@ -308,9 +308,6 @@
   </si>
   <si>
     <t>Gộp chung mạch</t>
-  </si>
-  <si>
-    <t>thiếu 1 cái</t>
   </si>
   <si>
     <t>chuyển USB vào chung mạch MCU, chuyển Micro SD vào mạch giải mã âm thanh</t>
@@ -519,6 +516,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,9 +530,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,7 +838,7 @@
   <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -874,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,10 +922,10 @@
       <c r="E4" s="14">
         <v>1</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
@@ -944,8 +941,8 @@
       <c r="E5" s="14">
         <v>1</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
@@ -1223,7 +1220,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="7"/>
+      <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
@@ -1238,7 +1235,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G22" s="7"/>
     </row>
@@ -1256,10 +1253,10 @@
       <c r="E23" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="G23" s="28"/>
+      <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
@@ -1273,8 +1270,8 @@
       <c r="E24" s="14">
         <v>1</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="28"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="24"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
@@ -1306,7 +1303,7 @@
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
@@ -1322,10 +1319,8 @@
       <c r="E27" s="14">
         <v>2</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G27" s="7"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="23"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
@@ -1359,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="23"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
@@ -1376,7 +1371,7 @@
         <v>2</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="7"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
@@ -1393,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="5"/>
-      <c r="G31" s="7"/>
+      <c r="G31" s="23"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
@@ -1410,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="5"/>
-      <c r="G32" s="7"/>
+      <c r="G32" s="23"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
@@ -1429,7 +1424,7 @@
       <c r="F33" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
@@ -1446,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="5"/>
-      <c r="G34" s="7"/>
+      <c r="G34" s="23"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
@@ -1480,7 +1475,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="5"/>
-      <c r="G36" s="7"/>
+      <c r="G36" s="23"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
@@ -1516,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="5"/>
-      <c r="G38" s="7"/>
+      <c r="G38" s="23"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
@@ -1606,14 +1601,14 @@
       <c r="G43" s="7"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="26"/>
-      <c r="C45" s="26"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="24" t="s">
+      <c r="B46" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="24"/>
+      <c r="C46" s="25"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
@@ -1649,17 +1644,17 @@
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="25"/>
+      <c r="C52" s="26"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="25">
+      <c r="B53" s="26">
         <f>1.23*(1+(C51/B51))</f>
         <v>2.73</v>
       </c>
-      <c r="C53" s="25"/>
+      <c r="C53" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>